<commit_message>
Update task checar MCM.
</commit_message>
<xml_diff>
--- a/_extrafiles/APROVADORES_PCP_FABRICADOS.xlsx
+++ b/_extrafiles/APROVADORES_PCP_FABRICADOS.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,13 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
-  <si>
-    <t>CIRINA77</t>
-  </si>
-  <si>
-    <t>ELTOBORG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>VWL</t>
   </si>
@@ -149,7 +143,19 @@
     <t>Aline</t>
   </si>
   <si>
-    <t>Elton</t>
+    <t>NADEFERR</t>
+  </si>
+  <si>
+    <t>CIRINA14</t>
+  </si>
+  <si>
+    <t>TENNECO</t>
+  </si>
+  <si>
+    <t>TENNECO BR</t>
+  </si>
+  <si>
+    <t>Nadevir</t>
   </si>
 </sst>
 </file>
@@ -174,13 +180,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,300 +487,315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>40</v>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D20">
+  <autoFilter ref="A1:D19">
     <sortState ref="A2:D20">
       <sortCondition ref="D1:D20"/>
     </sortState>

</xml_diff>